<commit_message>
Opdaterede lidt flere signaltyper i excelarket
</commit_message>
<xml_diff>
--- a/Way/WayObjects/Rail Signals/Signal Overview.xlsx
+++ b/Way/WayObjects/Rail Signals/Signal Overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\1993m\Documents\GitHub\Pak128.Nordic\Way\WayObjects\Rail Signals\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CE74A12-8583-40FF-8B8A-89A92589ADBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB8D3AF8-223C-4B05-9261-7D4AA43633AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="241">
   <si>
     <t>eksempel</t>
   </si>
@@ -683,9 +683,6 @@
     <t>Choose Signal</t>
   </si>
   <si>
-    <t>Stationsbestyrer</t>
-  </si>
-  <si>
     <t>Stop = vandret arm/rød, kør = skråt opad/hvid</t>
   </si>
   <si>
@@ -710,9 +707,6 @@
     <t>Stop = skive vises/grøn, kør = skive drejet op/hvid</t>
   </si>
   <si>
-    <t>Stop = vandre arm/gul, kør = skråt opad/grøn</t>
-  </si>
-  <si>
     <t>Banevogter med telegraf</t>
   </si>
   <si>
@@ -737,13 +731,25 @@
     <t>600 meter</t>
   </si>
   <si>
-    <t>2 km</t>
-  </si>
-  <si>
     <t xml:space="preserve">se de Danske Jernbaners Signaler side 30, 49, 52-53, </t>
   </si>
   <si>
     <t>Billeder af signalhuse side 10, 16, 21, 31, 41, 44-47, 59 osv</t>
+  </si>
+  <si>
+    <t>1000 meter</t>
+  </si>
+  <si>
+    <t>Stop = vandret arm/gul, kør = skråt opad/grøn</t>
+  </si>
+  <si>
+    <t>Stop = vandret arm/rød, kør = skråt opad/grøn</t>
+  </si>
+  <si>
+    <t>Trådtræk</t>
+  </si>
+  <si>
+    <t>Trådtræk, DSB1912</t>
   </si>
 </sst>
 </file>
@@ -803,17 +809,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
@@ -1172,7 +1174,7 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="4" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1271,10 +1273,10 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="1" t="s">
         <v>78</v>
       </c>
       <c r="C10" t="s">
@@ -1285,17 +1287,17 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="1" t="s">
         <v>83</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1445,10 +1447,10 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="1" t="s">
         <v>90</v>
       </c>
       <c r="D25" t="s">
@@ -1456,10 +1458,10 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D26" t="s">
@@ -1467,10 +1469,10 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="1" t="s">
         <v>107</v>
       </c>
       <c r="D27" t="s">
@@ -1478,10 +1480,10 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="1" t="s">
         <v>111</v>
       </c>
       <c r="D28" t="s">
@@ -1489,10 +1491,10 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="1" t="s">
         <v>114</v>
       </c>
       <c r="D29" s="3" t="s">
@@ -1500,35 +1502,35 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D30" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
+      <c r="A31" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D31" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" t="s">
         <v>125</v>
       </c>
     </row>
@@ -1690,13 +1692,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1708,15 +1710,15 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="4" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="1" t="s">
         <v>139</v>
       </c>
       <c r="D2" t="s">
@@ -1725,15 +1727,15 @@
       <c r="G2" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="4" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="1" t="s">
         <v>140</v>
       </c>
       <c r="D3" t="s">
@@ -1741,10 +1743,10 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="1" t="s">
         <v>141</v>
       </c>
       <c r="D4" t="s">
@@ -1752,10 +1754,10 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D5" t="s">
@@ -1763,10 +1765,10 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D6" t="s">
@@ -1774,10 +1776,10 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D7" t="s">
@@ -1785,10 +1787,10 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D8" t="s">
@@ -1796,10 +1798,10 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D9" t="s">
@@ -1807,10 +1809,10 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="1" t="s">
         <v>142</v>
       </c>
       <c r="D10" t="s">
@@ -1818,10 +1820,10 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D11" t="s">
@@ -1829,10 +1831,10 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="1" t="s">
         <v>88</v>
       </c>
       <c r="C12" t="s">
@@ -1843,10 +1845,10 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="1" t="s">
         <v>143</v>
       </c>
       <c r="C13" t="s">
@@ -1857,10 +1859,10 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="1" t="s">
         <v>132</v>
       </c>
       <c r="C14" t="s">
@@ -1871,10 +1873,10 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="1" t="s">
         <v>144</v>
       </c>
       <c r="D15" t="s">
@@ -1882,10 +1884,10 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="1" t="s">
         <v>111</v>
       </c>
       <c r="C16" t="s">
@@ -1896,10 +1898,10 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="1" t="s">
         <v>46</v>
       </c>
       <c r="C17" t="s">
@@ -1910,10 +1912,10 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="1" t="s">
         <v>145</v>
       </c>
       <c r="C18" t="s">
@@ -1924,10 +1926,10 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="1" t="s">
         <v>146</v>
       </c>
       <c r="C19" t="s">
@@ -1938,7 +1940,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="1" t="s">
         <v>157</v>
       </c>
     </row>
@@ -1953,10 +1955,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{517288DF-DC8F-4E11-9F1F-0BC1FADFFFC5}">
-  <dimension ref="A1:M38"/>
+  <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1974,12 +1976,12 @@
         <v>158</v>
       </c>
       <c r="H1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="H2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -2011,7 +2013,7 @@
         <v>187</v>
       </c>
       <c r="J4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="K4" t="s">
         <v>172</v>
@@ -2052,9 +2054,9 @@
         <v>188</v>
       </c>
       <c r="J5" t="s">
-        <v>231</v>
-      </c>
-      <c r="K5" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="K5" s="5" t="s">
         <v>204</v>
       </c>
       <c r="L5" t="s">
@@ -2090,9 +2092,9 @@
         <v>189</v>
       </c>
       <c r="J6" t="s">
-        <v>231</v>
-      </c>
-      <c r="K6" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="K6" s="5" t="s">
         <v>204</v>
       </c>
       <c r="L6" t="s">
@@ -2128,9 +2130,9 @@
         <v>191</v>
       </c>
       <c r="J7" t="s">
-        <v>231</v>
-      </c>
-      <c r="K7" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="K7" s="5" t="s">
         <v>205</v>
       </c>
       <c r="L7" t="s">
@@ -2169,9 +2171,9 @@
         <v>192</v>
       </c>
       <c r="J8" t="s">
-        <v>231</v>
-      </c>
-      <c r="K8" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="K8" s="5" t="s">
         <v>205</v>
       </c>
       <c r="L8" t="s">
@@ -2207,9 +2209,9 @@
         <v>171</v>
       </c>
       <c r="J9" t="s">
-        <v>231</v>
-      </c>
-      <c r="K9" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="K9" s="5" t="s">
         <v>205</v>
       </c>
       <c r="L9" t="s">
@@ -2239,7 +2241,7 @@
         <v>3</v>
       </c>
       <c r="G10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H10" t="s">
         <v>171</v>
@@ -2248,9 +2250,9 @@
         <v>201</v>
       </c>
       <c r="J10" t="s">
-        <v>231</v>
-      </c>
-      <c r="K10" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="K10" s="5" t="s">
         <v>205</v>
       </c>
       <c r="L10" t="s">
@@ -2280,7 +2282,7 @@
         <v>2</v>
       </c>
       <c r="G11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H11" t="s">
         <v>171</v>
@@ -2289,9 +2291,9 @@
         <v>200</v>
       </c>
       <c r="J11" t="s">
-        <v>231</v>
-      </c>
-      <c r="K11" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="K11" s="5" t="s">
         <v>205</v>
       </c>
       <c r="L11" t="s">
@@ -2321,15 +2323,15 @@
         <v>2</v>
       </c>
       <c r="G12" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H12" t="s">
         <v>183</v>
       </c>
       <c r="J12" t="s">
-        <v>232</v>
-      </c>
-      <c r="K12" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="K12" s="5" t="s">
         <v>182</v>
       </c>
       <c r="L12" t="s">
@@ -2362,9 +2364,9 @@
         <v>183</v>
       </c>
       <c r="J13" t="s">
-        <v>232</v>
-      </c>
-      <c r="K13" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="K13" s="5" t="s">
         <v>182</v>
       </c>
       <c r="L13" t="s">
@@ -2397,9 +2399,9 @@
         <v>183</v>
       </c>
       <c r="J14" t="s">
-        <v>232</v>
-      </c>
-      <c r="K14" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="K14" s="5" t="s">
         <v>182</v>
       </c>
       <c r="L14" t="s">
@@ -2438,9 +2440,9 @@
         <v>190</v>
       </c>
       <c r="J15" t="s">
-        <v>231</v>
-      </c>
-      <c r="K15" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="K15" s="5" t="s">
         <v>205</v>
       </c>
       <c r="L15" t="s">
@@ -2476,9 +2478,9 @@
         <v>193</v>
       </c>
       <c r="J16" t="s">
-        <v>231</v>
-      </c>
-      <c r="K16" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="K16" s="5" t="s">
         <v>205</v>
       </c>
       <c r="L16" t="s">
@@ -2517,9 +2519,9 @@
         <v>194</v>
       </c>
       <c r="J17" t="s">
-        <v>231</v>
-      </c>
-      <c r="K17" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="K17" s="5" t="s">
         <v>205</v>
       </c>
       <c r="L17" t="s">
@@ -2530,10 +2532,10 @@
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K18" s="7"/>
+      <c r="K18" s="5"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K19" s="7"/>
+      <c r="K19" s="5"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -2557,21 +2559,21 @@
       <c r="G20" t="s">
         <v>198</v>
       </c>
-      <c r="K20" s="8" t="s">
+      <c r="K20" s="6" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K21" s="7"/>
+      <c r="K21" s="5"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K22" s="7"/>
+      <c r="K22" s="5"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K23" s="7"/>
+      <c r="K23" s="5"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K24" s="7"/>
+      <c r="K24" s="5"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -2599,9 +2601,9 @@
         <v>207</v>
       </c>
       <c r="J25" t="s">
-        <v>234</v>
-      </c>
-      <c r="K25" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="K25" s="5" t="s">
         <v>208</v>
       </c>
       <c r="L25" t="s">
@@ -2637,10 +2639,10 @@
         <v>210</v>
       </c>
       <c r="J26" t="s">
-        <v>234</v>
-      </c>
-      <c r="K26" s="7" t="s">
-        <v>228</v>
+        <v>232</v>
+      </c>
+      <c r="K26" s="5" t="s">
+        <v>226</v>
       </c>
       <c r="L26" t="s">
         <v>175</v>
@@ -2656,11 +2658,14 @@
       <c r="B27">
         <v>1876</v>
       </c>
+      <c r="C27">
+        <v>1903</v>
+      </c>
       <c r="D27" t="s">
         <v>214</v>
       </c>
       <c r="E27" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F27">
         <v>2</v>
@@ -2672,92 +2677,92 @@
         <v>183</v>
       </c>
       <c r="J27" t="s">
-        <v>234</v>
-      </c>
-      <c r="K27" s="7" t="s">
-        <v>228</v>
+        <v>232</v>
+      </c>
+      <c r="K27" s="5" t="s">
+        <v>226</v>
       </c>
       <c r="L27" t="s">
         <v>176</v>
       </c>
       <c r="M27" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B28">
-        <v>1862</v>
+        <v>1881</v>
       </c>
       <c r="C28">
-        <v>1876</v>
+        <v>1903</v>
       </c>
       <c r="D28" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="E28" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="F28">
         <v>2</v>
       </c>
       <c r="G28" t="s">
-        <v>169</v>
+        <v>220</v>
       </c>
       <c r="H28" t="s">
-        <v>210</v>
+        <v>183</v>
       </c>
       <c r="J28" t="s">
-        <v>234</v>
-      </c>
-      <c r="K28" s="7" t="s">
-        <v>228</v>
+        <v>236</v>
+      </c>
+      <c r="K28" s="5" t="s">
+        <v>239</v>
       </c>
       <c r="L28" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="M28" t="s">
-        <v>212</v>
+        <v>225</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B29">
-        <v>1862</v>
+        <v>1883</v>
       </c>
       <c r="C29">
-        <v>1890</v>
+        <v>1903</v>
       </c>
       <c r="D29" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E29" t="s">
-        <v>216</v>
+        <v>181</v>
       </c>
       <c r="F29">
         <v>2</v>
       </c>
       <c r="G29" t="s">
-        <v>217</v>
+        <v>169</v>
       </c>
       <c r="H29" t="s">
         <v>183</v>
       </c>
       <c r="J29" t="s">
-        <v>234</v>
-      </c>
-      <c r="K29" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="K29" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="L29" t="s">
+        <v>176</v>
+      </c>
+      <c r="M29" t="s">
         <v>218</v>
-      </c>
-      <c r="L29" t="s">
-        <v>178</v>
-      </c>
-      <c r="M29" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
@@ -2765,51 +2770,54 @@
         <v>211</v>
       </c>
       <c r="B30">
-        <v>1870</v>
+        <v>1862</v>
       </c>
       <c r="C30">
-        <v>1890</v>
+        <v>1876</v>
       </c>
       <c r="D30" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="E30" t="s">
-        <v>197</v>
+        <v>206</v>
       </c>
       <c r="F30">
         <v>2</v>
       </c>
       <c r="G30" t="s">
-        <v>221</v>
+        <v>169</v>
       </c>
       <c r="H30" t="s">
-        <v>183</v>
+        <v>210</v>
       </c>
       <c r="J30" t="s">
-        <v>235</v>
-      </c>
-      <c r="K30" s="7" t="s">
-        <v>218</v>
+        <v>232</v>
+      </c>
+      <c r="K30" s="5" t="s">
+        <v>226</v>
       </c>
       <c r="L30" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="M30" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="B31">
+        <v>1862</v>
+      </c>
+      <c r="C31">
         <v>1890</v>
       </c>
       <c r="D31" t="s">
         <v>215</v>
       </c>
       <c r="E31" t="s">
-        <v>181</v>
+        <v>216</v>
       </c>
       <c r="F31">
         <v>2</v>
@@ -2821,74 +2829,77 @@
         <v>183</v>
       </c>
       <c r="J31" t="s">
-        <v>236</v>
-      </c>
-      <c r="K31" s="7" t="s">
-        <v>218</v>
+        <v>232</v>
+      </c>
+      <c r="K31" s="5" t="s">
+        <v>239</v>
       </c>
       <c r="L31" t="s">
         <v>178</v>
       </c>
       <c r="M31" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="B32">
-        <v>1903</v>
+        <v>1870</v>
+      </c>
+      <c r="C32">
+        <v>1890</v>
       </c>
       <c r="D32" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="E32" t="s">
-        <v>181</v>
+        <v>197</v>
       </c>
       <c r="F32">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G32" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="H32" t="s">
         <v>183</v>
       </c>
       <c r="J32" t="s">
-        <v>236</v>
-      </c>
-      <c r="K32" s="7" t="s">
-        <v>218</v>
+        <v>233</v>
+      </c>
+      <c r="K32" s="5" t="s">
+        <v>239</v>
       </c>
       <c r="L32" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M32" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>209</v>
+        <v>222</v>
       </c>
       <c r="B33">
-        <v>1881</v>
+        <v>1890</v>
       </c>
       <c r="C33">
         <v>1903</v>
       </c>
       <c r="D33" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="E33" t="s">
-        <v>197</v>
+        <v>181</v>
       </c>
       <c r="F33">
         <v>2</v>
       </c>
       <c r="G33" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="H33" t="s">
         <v>183</v>
@@ -2896,34 +2907,34 @@
       <c r="J33" t="s">
         <v>236</v>
       </c>
-      <c r="K33" s="7" t="s">
-        <v>218</v>
+      <c r="K33" s="5" t="s">
+        <v>239</v>
       </c>
       <c r="L33" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="M33" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B34">
         <v>1903</v>
       </c>
       <c r="D34" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="E34" t="s">
         <v>181</v>
       </c>
       <c r="F34">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G34" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="H34" t="s">
         <v>183</v>
@@ -2931,27 +2942,94 @@
       <c r="J34" t="s">
         <v>236</v>
       </c>
-      <c r="K34" s="7" t="s">
-        <v>218</v>
+      <c r="K34" s="5" t="s">
+        <v>240</v>
       </c>
       <c r="L34" t="s">
+        <v>177</v>
+      </c>
+      <c r="M34" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>222</v>
+      </c>
+      <c r="B35">
+        <v>1903</v>
+      </c>
+      <c r="D35" t="s">
+        <v>219</v>
+      </c>
+      <c r="E35" t="s">
+        <v>181</v>
+      </c>
+      <c r="F35">
+        <v>2</v>
+      </c>
+      <c r="G35" t="s">
+        <v>220</v>
+      </c>
+      <c r="H35" t="s">
+        <v>183</v>
+      </c>
+      <c r="J35" t="s">
+        <v>236</v>
+      </c>
+      <c r="K35" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="L35" t="s">
         <v>176</v>
       </c>
-      <c r="M34" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K35" s="7"/>
+      <c r="M35" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K36" s="7"/>
+      <c r="A36" t="s">
+        <v>222</v>
+      </c>
+      <c r="B36">
+        <v>1903</v>
+      </c>
+      <c r="D36" t="s">
+        <v>214</v>
+      </c>
+      <c r="E36" t="s">
+        <v>181</v>
+      </c>
+      <c r="F36">
+        <v>2</v>
+      </c>
+      <c r="G36" t="s">
+        <v>169</v>
+      </c>
+      <c r="H36" t="s">
+        <v>183</v>
+      </c>
+      <c r="J36" t="s">
+        <v>236</v>
+      </c>
+      <c r="K36" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="L36" t="s">
+        <v>176</v>
+      </c>
+      <c r="M36" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K37" s="7"/>
+      <c r="K37" s="5"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K38" s="7"/>
+      <c r="K38" s="5"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K39" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Tilføjede et dansk signal (AM2)
Første danske signal tilføjet
</commit_message>
<xml_diff>
--- a/Way/WayObjects/Rail Signals/Signal Overview.xlsx
+++ b/Way/WayObjects/Rail Signals/Signal Overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\1993m\Documents\GitHub\Pak128.Nordic\Way\WayObjects\Rail Signals\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92D6BA4E-A4B2-4CCD-9AAE-3D80153C1621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF0EB0E5-88BF-4B98-AA02-4B966DB87A73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="283">
   <si>
     <t>eksempel</t>
   </si>
@@ -870,6 +870,12 @@
   </si>
   <si>
     <t>Langå, Hillerød, Hjørring, Struer</t>
+  </si>
+  <si>
+    <t>Stationsgrænse?</t>
+  </si>
+  <si>
+    <t>End of choose</t>
   </si>
 </sst>
 </file>
@@ -2086,8 +2092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{517288DF-DC8F-4E11-9F1F-0BC1FADFFFC5}">
   <dimension ref="A1:M63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="L38" sqref="L38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3310,6 +3316,15 @@
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>281</v>
+      </c>
+      <c r="E38" t="s">
+        <v>195</v>
+      </c>
+      <c r="G38" t="s">
+        <v>282</v>
+      </c>
       <c r="K38" s="5"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>